<commit_message>
docs: Add results for v1
</commit_message>
<xml_diff>
--- a/Physik/Praktikum/Versuch Oberflächenspannung/Ergebnisse.xlsx
+++ b/Physik/Praktikum/Versuch Oberflächenspannung/Ergebnisse.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bwedu-my.sharepoint.com/personal/moritz_wieland_bwedu_de/Documents/Module/Physik/Praktikum/Versuch Oberflächenspannung/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moritz/git/university/Physik/Praktikum/Versuch Oberflächenspannung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="487" documentId="8_{E0FA83E2-246F-5344-AD71-71693061F64E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69E62AA9-F923-8C4E-B245-78746A31437C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5627D406-37A1-094F-BF98-2762C3EC5116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{DE81842C-0F6B-3545-A67E-92498C59F6F7}"/>
+    <workbookView xWindow="4860" yWindow="21600" windowWidth="28800" windowHeight="18000" xr2:uid="{DE81842C-0F6B-3545-A67E-92498C59F6F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -233,13 +233,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5434,8 +5433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A9E4F2-E95D-9E49-9C76-20B482CC2A84}">
   <dimension ref="A3:AO47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5466,8 +5465,6 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
docs: update protocol, add v3 and some minor changes
</commit_message>
<xml_diff>
--- a/Physik/Praktikum/Versuch Oberflächenspannung/Ergebnisse.xlsx
+++ b/Physik/Praktikum/Versuch Oberflächenspannung/Ergebnisse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moritz/git/university/Physik/Praktikum/Versuch Oberflächenspannung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5627D406-37A1-094F-BF98-2762C3EC5116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB196203-82E0-7540-9254-13B0C0530A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="21600" windowWidth="28800" windowHeight="18000" xr2:uid="{DE81842C-0F6B-3545-A67E-92498C59F6F7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26080" windowHeight="18000" xr2:uid="{DE81842C-0F6B-3545-A67E-92498C59F6F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,9 +107,6 @@
     <t>log c</t>
   </si>
   <si>
-    <t>Sigma(mN/m)</t>
-  </si>
-  <si>
     <t>mM</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   <si>
     <t>m4</t>
   </si>
+  <si>
+    <t>Sigma (mN/m)</t>
+  </si>
 </sst>
 </file>
 
@@ -270,37 +270,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -315,7 +285,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Sigma(mN/m)</c:v>
+                  <c:v>Sigma (mN/m)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -471,6 +441,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>log(c)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -533,6 +558,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Sigma</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (mN/m)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -671,37 +756,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -880,6 +935,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>1/r</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> [1/mm]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -942,6 +1057,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Höhe</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> [mm]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -991,6 +1166,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1049,37 +1255,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1258,6 +1434,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>1/r</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> [1/mm]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1320,6 +1556,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Höhe [mm]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1369,6 +1660,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1427,37 +1749,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1636,6 +1928,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>1/r [1/mm]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1698,6 +2045,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Höhe [mm]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1747,6 +2149,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1805,37 +2238,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -2014,6 +2417,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>1/r [1/mm]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2076,6 +2534,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Höhe</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> [mm]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2125,6 +2642,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -5433,8 +5981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A9E4F2-E95D-9E49-9C76-20B482CC2A84}">
   <dimension ref="A3:AO47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView tabSelected="1" topLeftCell="AB10" workbookViewId="0">
+      <selection activeCell="AK44" sqref="AK44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5542,10 +6090,10 @@
         <v>20</v>
       </c>
       <c r="R4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>21</v>
@@ -5554,37 +6102,37 @@
         <v>22</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="AD4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AG4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG4" s="1" t="s">
+      <c r="AJ4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI4" s="1" t="s">
+      <c r="AL4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AL4" s="1" t="s">
+      <c r="AM4" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="AM4" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.2">
@@ -5609,7 +6157,7 @@
         <v>0</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V5" s="1">
         <f>Q5/(2*PI()*$I$4)*1000</f>
@@ -6034,7 +6582,7 @@
         <v>50.525378759331851</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AL11" s="1">
         <f>283.03/50</f>
@@ -6045,7 +6593,7 @@
         <v>6.38</v>
       </c>
       <c r="AO11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.2">
@@ -6096,7 +6644,7 @@
         <v>42.946571945432076</v>
       </c>
       <c r="AD12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.2">
@@ -6175,7 +6723,7 @@
         <v>32.841496193565703</v>
       </c>
       <c r="AM14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.2">
@@ -6224,7 +6772,7 @@
         <v>38.525601303990534</v>
       </c>
       <c r="AH15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AM15" s="1">
         <v>15.936999999999999</v>
@@ -6364,7 +6912,7 @@
         <v>4</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P20" s="1">
         <f>U14</f>
@@ -6373,22 +6921,22 @@
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.2">
       <c r="O21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P21" s="1">
         <f>T14</f>
         <v>8.3333333333333339</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.2">
       <c r="AH28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AM28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.2">
@@ -6404,10 +6952,10 @@
         <v>0</v>
       </c>
       <c r="AF43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH43" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="AH43" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="44" spans="30:36" x14ac:dyDescent="0.2">
@@ -6415,13 +6963,13 @@
         <v>9.81</v>
       </c>
       <c r="AE44" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AF44" s="1">
         <v>0.997</v>
       </c>
       <c r="AG44" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AH44" s="1">
         <f>1/2*AH16*$AF$44*$AD$44</f>
@@ -6431,7 +6979,7 @@
         <v>4</v>
       </c>
       <c r="AJ44" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="30:36" x14ac:dyDescent="0.2">
@@ -6443,7 +6991,7 @@
         <v>4</v>
       </c>
       <c r="AJ45" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="30:36" x14ac:dyDescent="0.2">
@@ -6455,7 +7003,7 @@
         <v>4</v>
       </c>
       <c r="AJ46" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="30:36" x14ac:dyDescent="0.2">
@@ -6467,7 +7015,7 @@
         <v>4</v>
       </c>
       <c r="AJ47" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>